<commit_message>
Get detailed bulk request
</commit_message>
<xml_diff>
--- a/bulk-service/src/excelFilesExample/changeRoleHierarchyBulkExample.xlsx
+++ b/bulk-service/src/excelFilesExample/changeRoleHierarchyBulkExample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t xml:space="preserve">יוזר (TXXXXXX)</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">T5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מתכנת5</t>
   </si>
   <si>
     <t xml:space="preserve">ליצן5</t>
@@ -290,12 +293,14 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -438,7 +443,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,10 +481,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,10 +578,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -646,8 +647,11 @@
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,42 +691,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:L15"/>
+  <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.5"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="196" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="11" t="s">
-        <v>18</v>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>19</v>
+      <c r="A6" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,76 +736,76 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>20</v>
+      <c r="A8" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>23</v>
+      <c r="A9" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>25</v>
+      <c r="A10" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>27</v>
+      <c r="A11" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
-        <v>29</v>
+      <c r="A12" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>32</v>
+      <c r="A13" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>34</v>
+      <c r="A14" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>36</v>
+      <c r="A15" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>